<commit_message>
model export fixes + slider battery and slider winfarm addition to generic excel templates
</commit_message>
<xml_diff>
--- a/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
+++ b/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Brainport\data_Ekkersrijt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222E8DD5-EC8E-4804-8E5E-BC37D5340172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB43C208-A9D0-4A56-841E-27959A11E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>polygon</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>initially_active</t>
+  </si>
+  <si>
+    <t>SLIDER_GB</t>
+  </si>
+  <si>
+    <t>SLIDER_GB_Owner</t>
+  </si>
+  <si>
+    <t>NODAL_PRICING</t>
   </si>
 </sst>
 </file>
@@ -956,15 +965,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A76AC-78CE-4B58-B551-1045CBA11955}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
@@ -1048,6 +1057,44 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:20" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>5000</v>
+      </c>
+      <c r="O2">
+        <v>5000</v>
+      </c>
+      <c r="P2">
+        <v>5000</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2">
+        <v>52</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
trafo_id -> gridnode_id refactor
</commit_message>
<xml_diff>
--- a/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
+++ b/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Brainport\data_Ekkersrijt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB43C208-A9D0-4A56-841E-27959A11E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7143B92-B3EC-43C8-A243-1A671E3ED619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,9 +576,6 @@
     <t>storage_capacity_kwh</t>
   </si>
   <si>
-    <t>trafo_id</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -616,6 +613,9 @@
   </si>
   <si>
     <t>NODAL_PRICING</t>
+  </si>
+  <si>
+    <t>gridnode_id</t>
   </si>
 </sst>
 </file>
@@ -968,7 +968,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -997,37 +997,37 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="2" spans="1:20" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         <v>5000</v>
       </c>
       <c r="Q2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2">
         <v>52</v>

</xml_diff>

<commit_message>
removal of unnecessary slider gc in the battery and winfarm excel
</commit_message>
<xml_diff>
--- a/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
+++ b/data_Generic/data_ProjectTemplate/Batteries_ProjectTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7143B92-B3EC-43C8-A243-1A671E3ED619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FFE53E-02E8-4815-AF4E-054C475C8E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39540" yWindow="1140" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batteries" sheetId="2" r:id="rId1"/>
@@ -547,7 +547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>polygon</t>
   </si>
@@ -604,15 +604,6 @@
   </si>
   <si>
     <t>initially_active</t>
-  </si>
-  <si>
-    <t>SLIDER_GB</t>
-  </si>
-  <si>
-    <t>SLIDER_GB_Owner</t>
-  </si>
-  <si>
-    <t>NODAL_PRICING</t>
   </si>
   <si>
     <t>gridnode_id</t>
@@ -965,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29A76AC-78CE-4B58-B551-1045CBA11955}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1024,7 +1015,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>18</v>
@@ -1055,44 +1046,6 @@
       </c>
       <c r="T1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>5000</v>
-      </c>
-      <c r="O2">
-        <v>5000</v>
-      </c>
-      <c r="P2">
-        <v>5000</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2">
-        <v>52</v>
-      </c>
-      <c r="S2">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>